<commit_message>
Updates to Apportionment Weights
Here this is.
</commit_message>
<xml_diff>
--- a/threeWay_FE/stateCIT_rates_1976_2023.xlsx
+++ b/threeWay_FE/stateCIT_rates_1976_2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/Documents/GitHub/ST-Apportionment/threeWay_FE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3800DE68-1635-A743-BA66-572EF27CA0B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{768E015D-AD30-9F45-AFEE-8240944ED4FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15660" yWindow="-3100" windowWidth="15640" windowHeight="17500" xr2:uid="{902382AD-2791-2E4C-8E2C-F6478351B2FD}"/>
+    <workbookView xWindow="-32000" yWindow="-3100" windowWidth="32000" windowHeight="17500" xr2:uid="{902382AD-2791-2E4C-8E2C-F6478351B2FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -864,14 +864,14 @@
   <dimension ref="A1:AW51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AY6" sqref="AY6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="28" width="10.83203125" style="4" hidden="1" customWidth="1"/>
-    <col min="29" max="42" width="0" hidden="1" customWidth="1"/>
+    <col min="2" max="28" width="10.83203125" style="4" customWidth="1"/>
+    <col min="29" max="42" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:49">

</xml_diff>